<commit_message>
SCRUM Update E, G, H und I
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_F.xlsx
+++ b/SCRUM/SCRUM_TEAM_F.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -59,27 +59,15 @@
     <t>Implementierung der TicTacToe-Darstellung</t>
   </si>
   <si>
-    <t>Umsetzung des Painters im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung der TicTacToe-Regeln</t>
   </si>
   <si>
-    <t>Umsetzung der Rules im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung eines menschlichen TicTacToe-Spielers</t>
   </si>
   <si>
-    <t>Umsetzung eines menschlichen Players im Framework.</t>
-  </si>
-  <si>
     <t>Implementierung eines PC gesteurten TicTacToe-Spielers</t>
   </si>
   <si>
-    <t>Umsetzung eines PC gesteuerten Players im Framework.</t>
-  </si>
-  <si>
     <t>Spezifikation eines weiteren Spiels</t>
   </si>
   <si>
@@ -99,6 +87,33 @@
   </si>
   <si>
     <t>Due: 08.11.2021</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Umsetzung des Painters im Framework. Standard TicTacToe. Kreise und Kreuze. Darkmode. Ausblick: "Hidden-Modus": gesetzte Spielzüge verschwinden wieder.</t>
+  </si>
+  <si>
+    <t>Umsetzung der Rules im Framework. Standard TicTacToe. Ausblick: Zeitmodus: Timer läuft ab. Ausblick: Spieleinsatz.</t>
+  </si>
+  <si>
+    <t>Umsetzung eines menschlichen Players im Framework. Standard TicTacToe mit Mausbedingung. Ausblick: Spielername-Eingabe.</t>
+  </si>
+  <si>
+    <t>Umsetzung eines PC gesteuerten Players im Framework. Ausblick: Standard TicTacToe.</t>
+  </si>
+  <si>
+    <t>Focus Faktor: 0,5</t>
+  </si>
+  <si>
+    <t>240min</t>
+  </si>
+  <si>
+    <t>120min</t>
   </si>
 </sst>
 </file>
@@ -267,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -307,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -668,7 +686,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D6" s="13"/>
     </row>
@@ -677,10 +695,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7" s="13"/>
     </row>
@@ -689,10 +707,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8" s="13"/>
     </row>
@@ -701,10 +719,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D9" s="13"/>
     </row>
@@ -713,10 +731,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" s="13"/>
     </row>
@@ -725,10 +743,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="13"/>
     </row>
@@ -973,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,17 +1003,21 @@
     <col min="2" max="2" width="33.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="65.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="28.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1020,10 +1042,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1034,76 +1059,108 @@
         <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="13"/>
     </row>
-    <row r="10" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>

</xml_diff>